<commit_message>
Libreoffice Sheet/Named ranges and Expressions - Header, Sql1
</commit_message>
<xml_diff>
--- a/kupci_pregled_dugovanja_2.xlsx
+++ b/kupci_pregled_dugovanja_2.xlsx
@@ -11,8 +11,8 @@
     <sheet name="kupci_pregled_dugovanja" sheetId="1" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="false" name="Header" vbProcedure="false">kupci_pregled_dugovanja!$A$1:$I$1</definedName>
-    <definedName function="false" hidden="false" name="Sql1" vbProcedure="false">kupci_pregled_dugovanja!$A$2:$I$2</definedName>
+    <definedName function="false" hidden="false" name="Header" vbProcedure="false">kupci_pregled_dugovanja!$A$1:$L$1</definedName>
+    <definedName function="false" hidden="false" name="Sql1" vbProcedure="false">kupci_pregled_dugovanja!$A$2:$L$2</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="21">
   <si>
     <t xml:space="preserve">Konto Id</t>
   </si>
@@ -87,15 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">${i_ukupno}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${partn_vr_obezbj_naz}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${partn_velicina_naz}</t>
-  </si>
-  <si>
-    <t xml:space="preserve">${partn_regija_naz}</t>
   </si>
 </sst>
 </file>
@@ -237,7 +228,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -292,10 +283,6 @@
     </xf>
     <xf numFmtId="167" fontId="10" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="right" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="false" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="false" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
@@ -380,7 +367,7 @@
       <c r="AMI1" s="0"/>
       <c r="AMJ1" s="0"/>
     </row>
-    <row r="2" s="15" customFormat="true" ht="15.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="2" s="14" customFormat="true" ht="15.55" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="7" t="s">
         <v>12</v>
       </c>
@@ -408,14 +395,14 @@
       <c r="I2" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="J2" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" s="14" t="s">
-        <v>23</v>
+      <c r="J2" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="K2" s="8" t="s">
+        <v>13</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>14</v>
       </c>
       <c r="AMH2" s="0"/>
       <c r="AMI2" s="0"/>

</xml_diff>